<commit_message>
Created config, devide mqtt things, readme test
</commit_message>
<xml_diff>
--- a/public/Data/2_4_2020.xlsx
+++ b/public/Data/2_4_2020.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -433,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1522,6 +1522,46 @@
         <v>14</v>
       </c>
     </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43953.378890231485</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>43953.37916302083</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>